<commit_message>
Add principal/clerk semester promotion feature
</commit_message>
<xml_diff>
--- a/DATA FOR IMPORT EXPORT/BCA/BCA-Sem-1-Subject-list-with-code-1.xlsx
+++ b/DATA FOR IMPORT EXPORT/BCA/BCA-Sem-1-Subject-list-with-code-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\CMSv5\DATA FOR IMPORT EXPORT\BCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E05B28-D7CA-47C4-A061-665F299D9701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73642032-E3BC-4649-858E-7AF6A7ECD5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -493,19 +493,19 @@
       <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -563,7 +563,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -592,7 +592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -621,7 +621,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -650,7 +650,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -679,7 +679,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -708,7 +708,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -737,7 +737,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -766,7 +766,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -806,7 +806,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -818,7 +818,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>